<commit_message>
Made it slightly faster... again. Using some tricky hacks now
</commit_message>
<xml_diff>
--- a/running_time.xlsx
+++ b/running_time.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>MARS Tool Output</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>Version 2:</t>
+  </si>
+  <si>
+    <t>Version 3:</t>
   </si>
 </sst>
 </file>
@@ -229,7 +232,7 @@
   <dimension ref="A2:I21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -300,11 +303,11 @@
         <v>4319</v>
       </c>
       <c r="H6" s="0" t="n">
-        <v>1147</v>
+        <v>1925</v>
       </c>
       <c r="I6" s="0" t="n">
         <f aca="false">H6</f>
-        <v>1147</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -326,11 +329,11 @@
         <v>298</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I7" s="0" t="n">
         <f aca="false">H7</f>
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -352,11 +355,11 @@
         <v>2332</v>
       </c>
       <c r="H8" s="0" t="n">
-        <v>468</v>
+        <v>835</v>
       </c>
       <c r="I8" s="0" t="n">
         <f aca="false">H8 * 2</f>
-        <v>936</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -386,11 +389,11 @@
         <v>7950</v>
       </c>
       <c r="H10" s="0" t="n">
-        <v>460</v>
+        <v>91</v>
       </c>
       <c r="I10" s="0" t="n">
         <f aca="false">H10 * 5</f>
-        <v>2300</v>
+        <v>455</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -425,11 +428,11 @@
         <v>1022</v>
       </c>
       <c r="H14" s="0" t="n">
-        <v>303</v>
+        <v>315</v>
       </c>
       <c r="I14" s="0" t="n">
         <f aca="false">H14 * 2</f>
-        <v>606</v>
+        <v>630</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -451,11 +454,11 @@
         <v>16040</v>
       </c>
       <c r="H15" s="0" t="n">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="I15" s="0" t="n">
         <f aca="false"> H15 * 40</f>
-        <v>4520</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -465,7 +468,7 @@
       </c>
       <c r="I16" s="0" t="n">
         <f aca="false">SUM(I6:I15)</f>
-        <v>9832</v>
+        <v>9002</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -484,7 +487,14 @@
         <v>9832</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>9002</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>